<commit_message>
January 15, 2025 commit
</commit_message>
<xml_diff>
--- a/xlsxPCES/examples/embedded-model.xlsx
+++ b/xlsxPCES/examples/embedded-model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicol/Dropbox/github-repos/pcesbld-working/xlsxPCES/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicol/Dropbox/github-repos/pcesapps-working/embedded/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91C82A4-5E36-4D4E-A484-019C6B6104A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594D3D95-9FA1-4046-8BAC-83EC1F488FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="2920" windowWidth="24640" windowHeight="18040" activeTab="4" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
+    <workbookView xWindow="3360" yWindow="760" windowWidth="34560" windowHeight="20480" activeTab="1" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="topo" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="execTime" sheetId="4" r:id="rId3"/>
     <sheet name="mapping" sheetId="2" r:id="rId4"/>
     <sheet name="netParams" sheetId="5" r:id="rId5"/>
+    <sheet name="experiments" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="193">
   <si>
     <t>Networks</t>
   </si>
@@ -556,6 +557,66 @@
   </si>
   <si>
     <t>Wireless-Connections</t>
+  </si>
+  <si>
+    <t>exp-1</t>
+  </si>
+  <si>
+    <t>exp-2</t>
+  </si>
+  <si>
+    <t>AES-256-CBC</t>
+  </si>
+  <si>
+    <t>exp-3</t>
+  </si>
+  <si>
+    <t>AES-128-CBC</t>
+  </si>
+  <si>
+    <t>exp-4</t>
+  </si>
+  <si>
+    <t>Experiments</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>$crypto,cp</t>
+  </si>
+  <si>
+    <t>$bndwdth,netParams</t>
+  </si>
+  <si>
+    <t>encrypt-$crypto</t>
+  </si>
+  <si>
+    <t>decrypt-$crypto</t>
+  </si>
+  <si>
+    <t>$bndwdth</t>
+  </si>
+  <si>
+    <t>$zerotrust,cp</t>
+  </si>
+  <si>
+    <t>exp-5</t>
+  </si>
+  <si>
+    <t>exp-6</t>
+  </si>
+  <si>
+    <t>exp-7</t>
+  </si>
+  <si>
+    <t>exp-8</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>$zerotrust</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1196,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1148,6 +1209,9 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1525,7 +1589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95325CDA-052A-9A47-A8FD-348C19C2091E}">
   <dimension ref="A2:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
@@ -1860,10 +1924,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FA9935-1338-5743-9994-8B53C9940146}">
-  <dimension ref="A3:M101"/>
+  <dimension ref="A3:N100"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="150" workbookViewId="0">
-      <selection activeCell="K97" sqref="K97"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" zoomScaleNormal="164" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1877,10 +1941,11 @@
     <col min="7" max="7" width="21.1640625" customWidth="1"/>
     <col min="8" max="8" width="21.33203125" customWidth="1"/>
     <col min="9" max="9" width="20.1640625" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" customWidth="1"/>
     <col min="11" max="11" width="6.33203125" customWidth="1"/>
     <col min="12" max="12" width="21.33203125" customWidth="1"/>
-    <col min="13" max="14" width="24.33203125" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2310,12 +2375,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>85</v>
       </c>
@@ -2355,8 +2420,11 @@
       <c r="M52" s="5" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N52" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>75</v>
       </c>
@@ -2366,6 +2434,9 @@
       <c r="C53" t="s">
         <v>113</v>
       </c>
+      <c r="D53" t="s">
+        <v>192</v>
+      </c>
       <c r="F53" t="s">
         <v>57</v>
       </c>
@@ -2376,7 +2447,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>75</v>
       </c>
@@ -2386,6 +2457,9 @@
       <c r="C54" t="s">
         <v>113</v>
       </c>
+      <c r="D54" t="s">
+        <v>192</v>
+      </c>
       <c r="F54" t="s">
         <v>57</v>
       </c>
@@ -2396,7 +2470,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -2419,10 +2493,10 @@
         <v>114</v>
       </c>
       <c r="J55" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>75</v>
       </c>
@@ -2445,150 +2519,156 @@
         <v>114</v>
       </c>
       <c r="J56" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>75</v>
-      </c>
-      <c r="B57" t="s">
-        <v>110</v>
-      </c>
-      <c r="C57" t="s">
-        <v>113</v>
-      </c>
-      <c r="F57" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" t="s">
+        <v>105</v>
+      </c>
+      <c r="E59" t="s">
+        <v>117</v>
+      </c>
+      <c r="H59" t="s">
         <v>57</v>
       </c>
-      <c r="G57" t="s">
+      <c r="I59" t="s">
         <v>121</v>
       </c>
-      <c r="J57" t="s">
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" t="s">
+        <v>117</v>
+      </c>
+      <c r="D61" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B59" s="1" t="s">
+      <c r="E61" t="s">
+        <v>117</v>
+      </c>
+      <c r="H61" t="s">
+        <v>57</v>
+      </c>
+      <c r="I61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" t="s">
+        <v>114</v>
+      </c>
+      <c r="F63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F64" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D59" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="G59" s="1" t="s">
+      <c r="D66" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="G66" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="I59" s="5" t="s">
+      <c r="H66" s="5" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>77</v>
-      </c>
-      <c r="B60" t="s">
-        <v>118</v>
-      </c>
-      <c r="C60" t="s">
-        <v>117</v>
-      </c>
-      <c r="D60" t="s">
-        <v>105</v>
-      </c>
-      <c r="E60" t="s">
-        <v>117</v>
-      </c>
-      <c r="H60" t="s">
-        <v>57</v>
-      </c>
-      <c r="I60" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>77</v>
-      </c>
-      <c r="B62" t="s">
-        <v>116</v>
-      </c>
-      <c r="C62" t="s">
-        <v>117</v>
-      </c>
-      <c r="D62" t="s">
-        <v>105</v>
-      </c>
-      <c r="E62" t="s">
-        <v>117</v>
-      </c>
-      <c r="H62" t="s">
-        <v>57</v>
-      </c>
-      <c r="I62" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>77</v>
-      </c>
-      <c r="B64" t="s">
-        <v>112</v>
-      </c>
-      <c r="C64" t="s">
-        <v>114</v>
-      </c>
-      <c r="F64" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F65" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="H67" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I66" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67" t="s">
+        <v>106</v>
+      </c>
+      <c r="D67" t="s">
+        <v>122</v>
+      </c>
+      <c r="E67" t="s">
+        <v>31</v>
+      </c>
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>30</v>
       </c>
@@ -2596,356 +2676,351 @@
         <v>103</v>
       </c>
       <c r="C68" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="D68" t="s">
         <v>122</v>
       </c>
       <c r="E68" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="F68" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" t="s">
+        <v>103</v>
+      </c>
+      <c r="C72" t="s">
+        <v>104</v>
+      </c>
+      <c r="D72">
+        <v>1000</v>
+      </c>
+      <c r="E72">
+        <v>1500</v>
+      </c>
+      <c r="F72" t="s">
         <v>30</v>
       </c>
-      <c r="B69" t="s">
+      <c r="G72">
+        <v>10</v>
+      </c>
+      <c r="I72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>32</v>
+      </c>
+      <c r="B75" t="s">
         <v>103</v>
       </c>
-      <c r="C69" t="s">
-        <v>26</v>
-      </c>
-      <c r="D69" t="s">
-        <v>122</v>
-      </c>
-      <c r="E69" t="s">
-        <v>123</v>
-      </c>
-      <c r="F69" t="b">
+      <c r="C75" t="s">
+        <v>74</v>
+      </c>
+      <c r="D75" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B72" s="1" t="s">
+      <c r="E75" t="s">
+        <v>32</v>
+      </c>
+      <c r="F75" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I72" s="1" t="s">
+      <c r="D77" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>31</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="H77" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J79" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="K79" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="L79" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>33</v>
+      </c>
+      <c r="B80" t="s">
         <v>103</v>
       </c>
-      <c r="C73" t="s">
-        <v>104</v>
-      </c>
-      <c r="D73">
-        <v>1000</v>
-      </c>
-      <c r="E73">
-        <v>1500</v>
-      </c>
-      <c r="F73" t="s">
-        <v>30</v>
-      </c>
-      <c r="G73">
-        <v>10</v>
-      </c>
-      <c r="I73" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B75" s="1" t="s">
+      <c r="C80" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" t="s">
+        <v>115</v>
+      </c>
+      <c r="E80" t="s">
+        <v>128</v>
+      </c>
+      <c r="F80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>33</v>
+      </c>
+      <c r="B82" t="s">
+        <v>103</v>
+      </c>
+      <c r="C82" t="s">
+        <v>167</v>
+      </c>
+      <c r="D82" t="s">
+        <v>20</v>
+      </c>
+      <c r="E82" t="s">
+        <v>183</v>
+      </c>
+      <c r="F82" t="b">
+        <v>1</v>
+      </c>
+      <c r="I82" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>33</v>
+      </c>
+      <c r="B84" t="s">
+        <v>103</v>
+      </c>
+      <c r="C84" t="s">
+        <v>168</v>
+      </c>
+      <c r="D84" t="s">
+        <v>119</v>
+      </c>
+      <c r="E84" t="s">
+        <v>184</v>
+      </c>
+      <c r="F84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I84" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>33</v>
+      </c>
+      <c r="B86" t="s">
+        <v>103</v>
+      </c>
+      <c r="C86" t="s">
+        <v>108</v>
+      </c>
+      <c r="D86" t="s">
+        <v>120</v>
+      </c>
+      <c r="E86" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>33</v>
+      </c>
+      <c r="B88" t="s">
+        <v>110</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D88" t="s">
+        <v>120</v>
+      </c>
+      <c r="E88" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D92" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H92" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E75" s="5" t="s">
+      <c r="I92" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="F75" s="5" t="s">
+      <c r="J92" s="5" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>32</v>
-      </c>
-      <c r="B76" t="s">
-        <v>103</v>
-      </c>
-      <c r="C76" t="s">
-        <v>74</v>
-      </c>
-      <c r="D76" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" t="s">
-        <v>32</v>
-      </c>
-      <c r="F76" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H78" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="I78" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="H80" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J80" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="K80" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>33</v>
-      </c>
-      <c r="B81" t="s">
-        <v>103</v>
-      </c>
-      <c r="C81" t="s">
-        <v>107</v>
-      </c>
-      <c r="D81" t="s">
-        <v>115</v>
-      </c>
-      <c r="E81" t="s">
-        <v>128</v>
-      </c>
-      <c r="F81" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>33</v>
-      </c>
-      <c r="B83" t="s">
-        <v>103</v>
-      </c>
-      <c r="C83" t="s">
-        <v>167</v>
-      </c>
-      <c r="D83" t="s">
-        <v>20</v>
-      </c>
-      <c r="E83" t="s">
-        <v>129</v>
-      </c>
-      <c r="F83" t="b">
-        <v>1</v>
-      </c>
-      <c r="I83" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>33</v>
-      </c>
-      <c r="B85" t="s">
-        <v>103</v>
-      </c>
-      <c r="C85" t="s">
-        <v>168</v>
-      </c>
-      <c r="D85" t="s">
-        <v>119</v>
-      </c>
-      <c r="E85" t="s">
-        <v>130</v>
-      </c>
-      <c r="F85" t="b">
-        <v>1</v>
-      </c>
-      <c r="I85" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>33</v>
-      </c>
-      <c r="B87" t="s">
-        <v>103</v>
-      </c>
-      <c r="C87" t="s">
-        <v>108</v>
-      </c>
-      <c r="D87" t="s">
-        <v>120</v>
-      </c>
-      <c r="E87" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>33</v>
-      </c>
-      <c r="B89" t="s">
-        <v>110</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D89" t="s">
-        <v>120</v>
-      </c>
-      <c r="E89" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I93" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="J93" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+      <c r="K92" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="2" t="s">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
         <v>79</v>
       </c>
     </row>
+    <row r="97" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="98" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="11" t="s">
+      <c r="A98" s="11" t="s">
         <v>139</v>
       </c>
     </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" s="5" t="s">
+      <c r="A100" s="5" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2959,7 +3034,7 @@
   <dimension ref="A2:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3697,8 +3772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04436424-07DF-B343-BAAE-706A3CFD4756}">
   <dimension ref="A2:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3889,6 +3964,9 @@
       <c r="H18">
         <v>5</v>
       </c>
+      <c r="I18" t="s">
+        <v>185</v>
+      </c>
       <c r="K18" t="b">
         <v>0</v>
       </c>
@@ -3916,6 +3994,157 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD0BE0C2-6CFA-B544-AD1B-E0CD7C820A66}">
+  <dimension ref="A2:D11"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" s="12">
+        <v>10</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" s="12">
+        <v>10</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="12">
+        <v>10</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="12">
+        <v>10</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>